<commit_message>
chess template xlsx - cosmetic change Bishop movement - in MyBishop deletion of comments in MyPanel + modification of condition for clicking outside of board
</commit_message>
<xml_diff>
--- a/Java/szachy/Chess_board_template.xlsx
+++ b/Java/szachy/Chess_board_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tomek\Repositories\IT_development\Java\szachy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BFAE8D-78D6-4589-84E1-39F8B1CEED79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8276B8-AA3D-4ECF-BA7B-3ED3CC430390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CE5052A9-93DE-4E8D-9D63-A7BA867AB3BD}"/>
   </bookViews>
@@ -450,9 +450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2511B339-3BD5-4440-9974-CA6A6A602D21}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -562,7 +560,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="str">
-        <f t="shared" ref="C4:C10" si="1">""&amp;C$1&amp;","&amp;$A4</f>
+        <f t="shared" ref="C4:C9" si="1">""&amp;C$1&amp;","&amp;$A4</f>
         <v>0,1</v>
       </c>
       <c r="D4" s="1" t="str">
@@ -820,7 +818,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>""&amp;C$1&amp;","&amp;$A10</f>
         <v>0,7</v>
       </c>
       <c r="D10" s="1" t="str">

</xml_diff>